<commit_message>
referee spec with interruptions
</commit_message>
<xml_diff>
--- a/diagrams/referee/Referees.xlsx
+++ b/diagrams/referee/Referees.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\owlcms-firmata\diagrams\referee\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\owlcms-firmata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23DB394A-34B6-4D79-B9E5-1130443810CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B4CD67C-F546-4406-A582-D944C9C8DA83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{F9C8F068-60C0-4FDD-8C1E-880F519290ED}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{F9C8F068-60C0-4FDD-8C1E-880F519290ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Referee" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="48">
   <si>
     <t>pin</t>
   </si>
@@ -135,9 +135,6 @@
     <t>refbox/decision</t>
   </si>
   <si>
-    <t>1000 200 200</t>
-  </si>
-  <si>
     <t>TONE</t>
   </si>
   <si>
@@ -147,12 +144,6 @@
     <t>Down sound A1</t>
   </si>
   <si>
-    <t>C6,250,PAUSE,125,C6,250</t>
-  </si>
-  <si>
-    <t>C4,250,C5,250,PAUSE,250,C4,250,C5,250</t>
-  </si>
-  <si>
     <t>button</t>
   </si>
   <si>
@@ -171,13 +162,22 @@
     <t>ignore A5</t>
   </si>
   <si>
-    <t>D6,250,PAUSE,125,F6,250,PAUSE,125,G6,250</t>
-  </si>
-  <si>
-    <t>D5,250,PAUSE,125,F5,250,PAUSE,125,G5,250</t>
-  </si>
-  <si>
-    <t>A4,1000</t>
+    <t>1800,200,100 - 6,7</t>
+  </si>
+  <si>
+    <t>C6,250,D6,250,PAUSE,250,C6,250,D6,250</t>
+  </si>
+  <si>
+    <t>1800,200,100 - 3,2</t>
+  </si>
+  <si>
+    <t>1250,250,250</t>
+  </si>
+  <si>
+    <t>1800,200,100 - 10,11</t>
+  </si>
+  <si>
+    <t>fop/teststartup</t>
   </si>
 </sst>
 </file>
@@ -248,7 +248,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -318,8 +318,20 @@
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -636,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{593FC154-758F-4104-A30E-11A530E91792}">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -653,7 +665,8 @@
     <col min="7" max="7" width="10.85546875" style="4" customWidth="1"/>
     <col min="8" max="8" width="20.42578125" style="1" customWidth="1"/>
     <col min="9" max="9" width="9.140625" style="1"/>
-    <col min="10" max="16384" width="9.140625" style="5"/>
+    <col min="10" max="10" width="35.140625" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="17" customFormat="1" ht="15.75" thickBot="1">
@@ -664,7 +677,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D1" s="13" t="s">
         <v>8</v>
@@ -676,7 +689,7 @@
         <v>24</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H1" s="13" t="s">
         <v>1</v>
@@ -702,27 +715,27 @@
         <v>26</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="23">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -758,22 +771,22 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="23">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="30">
@@ -790,10 +803,10 @@
         <v>1</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -847,7 +860,7 @@
         <v>26</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="7"/>
@@ -855,22 +868,22 @@
     </row>
     <row r="11" spans="1:9" s="12" customFormat="1">
       <c r="A11" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B11" s="24">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" s="7">
         <v>2</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="G11" s="11"/>
       <c r="H11" s="7"/>
@@ -916,21 +929,21 @@
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
     </row>
-    <row r="14" spans="1:9" s="12" customFormat="1" ht="30">
+    <row r="14" spans="1:9" s="12" customFormat="1">
       <c r="A14" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D14" s="7">
         <v>2</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F14" s="10" t="s">
         <v>45</v>
@@ -953,10 +966,10 @@
         <v>2</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="G15" s="11"/>
       <c r="H15" s="7"/>
@@ -972,9 +985,7 @@
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="9"/>
-      <c r="F16" s="10" t="s">
-        <v>33</v>
-      </c>
+      <c r="F16" s="10"/>
       <c r="G16" s="11" t="s">
         <v>2</v>
       </c>
@@ -1023,18 +1034,18 @@
         <v>26</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" s="23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D19" s="1">
         <v>3</v>
@@ -1043,7 +1054,7 @@
         <v>26</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1060,66 +1071,67 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:9" s="29" customFormat="1">
+      <c r="A21" s="25" t="s">
         <v>18</v>
       </c>
       <c r="B21" s="23">
         <v>5</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F21" s="25">
+      <c r="D21" s="25"/>
+      <c r="E21" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" s="27">
         <v>1000</v>
       </c>
+      <c r="G21" s="28"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="23">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="30">
+        <v>26</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B23" s="23">
         <v>4</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" s="1">
-        <v>3</v>
+      <c r="C23" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="30">
+        <v>26</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B24" s="23">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>28</v>
@@ -1128,35 +1140,38 @@
         <v>3</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="30">
       <c r="A25" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B25" s="23">
+        <v>4</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="1">
         <v>3</v>
       </c>
-      <c r="G25" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>21</v>
+      <c r="E25" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B26" s="23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>2</v>
@@ -1165,36 +1180,32 @@
         <v>32</v>
       </c>
       <c r="I26" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="23">
+        <v>2</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I27" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" s="12" customFormat="1">
-      <c r="A27" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" s="23">
-        <v>14</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D27" s="7"/>
-      <c r="E27" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="F27" s="10">
-        <v>2000</v>
-      </c>
-      <c r="G27" s="11"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
     </row>
     <row r="28" spans="1:9" s="12" customFormat="1">
       <c r="A28" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B28" s="23">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>31</v>
@@ -1204,33 +1215,39 @@
         <v>2</v>
       </c>
       <c r="F28" s="10">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="G28" s="11"/>
       <c r="H28" s="7"/>
       <c r="I28" s="7"/>
     </row>
-    <row r="29" spans="1:9" customFormat="1">
-      <c r="A29" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="B29" s="19">
-        <v>16</v>
-      </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
+    <row r="29" spans="1:9" s="12" customFormat="1">
+      <c r="A29" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="23">
+        <v>15</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="7"/>
+      <c r="E29" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F29" s="10">
+        <v>1000</v>
+      </c>
+      <c r="G29" s="11"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
     </row>
     <row r="30" spans="1:9" customFormat="1">
       <c r="A30" s="18" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B30" s="19">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C30" s="18"/>
       <c r="D30" s="18"/>
@@ -1242,10 +1259,10 @@
     </row>
     <row r="31" spans="1:9" customFormat="1">
       <c r="A31" s="18" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B31" s="19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C31" s="18"/>
       <c r="D31" s="18"/>
@@ -1257,10 +1274,10 @@
     </row>
     <row r="32" spans="1:9" customFormat="1">
       <c r="A32" s="18" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B32" s="19">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C32" s="18"/>
       <c r="D32" s="18"/>
@@ -1270,7 +1287,25 @@
       <c r="H32" s="18"/>
       <c r="I32" s="18"/>
     </row>
+    <row r="33" spans="1:9" customFormat="1">
+      <c r="A33" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="19">
+        <v>19</v>
+      </c>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A18:I27">
+    <sortCondition ref="C18:C27"/>
+  </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>